<commit_message>
framework changed back to the previous one with xpath changes
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/TC_PA_008_To_TC_PA_022_errorScenarios.xlsx
+++ b/resources/ExcelsheetData/TC_PA_008_To_TC_PA_022_errorScenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prks\AppData\Roaming\Skype\My Skype Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UnilogProjects\etna\resources\ExcelsheetData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -240,10 +240,10 @@
     <t>tes</t>
   </si>
   <si>
-    <t>Password should have at least 8 characters</t>
-  </si>
-  <si>
     <t>Please enter Email Address.Please enter First Name.Please enter Last Name.Please enter Password.Please enter Confirm Password.Please enter Address 1Please enter City.Please select/enter State.Please enter Zipcode.Please enter Phone Number.</t>
+  </si>
+  <si>
+    <t>Password should have at least 8 characters.</t>
   </si>
 </sst>
 </file>
@@ -324,19 +324,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1501,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1613,7 +1614,7 @@
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1657,7 +1658,7 @@
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1701,7 +1702,7 @@
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1745,7 +1746,7 @@
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1789,7 +1790,7 @@
       </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1833,7 +1834,7 @@
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1877,7 +1878,7 @@
       </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="5" t="s">
+      <c r="P8" s="6" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1921,7 +1922,7 @@
       </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1965,7 +1966,7 @@
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
-      <c r="P10" s="5" t="s">
+      <c r="P10" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2009,12 +2010,12 @@
       </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
-      <c r="P11" s="5" t="s">
+      <c r="P11" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="4"/>
@@ -2031,12 +2032,12 @@
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
-      <c r="P12" s="7" t="s">
-        <v>71</v>
+      <c r="P12" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2077,12 +2078,12 @@
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="5" t="s">
+      <c r="P13" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2123,12 +2124,12 @@
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="3" t="s">
+      <c r="P14" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2169,12 +2170,12 @@
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="5" t="s">
+      <c r="P15" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -2215,12 +2216,12 @@
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="5" t="s">
-        <v>70</v>
+      <c r="P16" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2261,12 +2262,12 @@
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="5" t="s">
+      <c r="P17" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2307,7 +2308,7 @@
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
-      <c r="P18" s="5" t="s">
+      <c r="P18" s="6" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>